<commit_message>
updated default device tc
</commit_message>
<xml_diff>
--- a/PSPSProject/testData/testData.xlsx
+++ b/PSPSProject/testData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2B40AA-0607-44EA-9231-541074B75914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C2DF6E-1433-4861-8F38-80F3DF6F8913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>Execute</t>
   </si>
@@ -212,6 +212,21 @@
   </si>
   <si>
     <t>Device Cache Logic</t>
+  </si>
+  <si>
+    <t>CentralA01_1209R1</t>
+  </si>
+  <si>
+    <t>User specific_timeplaceName</t>
+  </si>
+  <si>
+    <t>Default Device Logic</t>
+  </si>
+  <si>
+    <t>Test_devicecheck</t>
+  </si>
+  <si>
+    <t>test_data_defaultdevicecheck.py</t>
   </si>
 </sst>
 </file>
@@ -740,7 +755,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1838,7 +1937,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D12" sqref="D12"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2389,130 +2488,130 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="71" priority="381" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="382" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="381" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="382" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="69" priority="379" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="380" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="379" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="380" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="67" priority="377" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="377" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="378" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="65" priority="375" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="376" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="375" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="376" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="63" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="59" priority="19" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="57" priority="17" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="55" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="16" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="53" priority="13" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2543,7 +2642,7 @@
   <dimension ref="A1:GV9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2615,7 +2714,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>9</v>
@@ -2665,9 +2764,33 @@
         <v>1</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:8" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="43">
+        <v>1</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="24"/>
@@ -2687,6 +2810,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="20" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2694,7 +2849,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2702,7 +2857,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2710,7 +2865,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2718,49 +2873,49 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A5" xr:uid="{97BE53CD-10F5-4B65-A481-D9129253028C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6" xr:uid="{97BE53CD-10F5-4B65-A481-D9129253028C}">
       <formula1>"Y,N,End"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CCDA7A78-A04D-4402-B991-2E5BCAB586CA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F6" xr:uid="{CCDA7A78-A04D-4402-B991-2E5BCAB586CA}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D5" xr:uid="{26455790-AA52-4327-A83D-3E6CDDE2F64E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D6" xr:uid="{26455790-AA52-4327-A83D-3E6CDDE2F64E}">
       <formula1>"Chrome-Default,Chrome-Headless,Chrome-MAC-Default,Chrome-MAC-Headless"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E5" xr:uid="{7DF67D48-D63D-43C5-9073-DA098A501C27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E6" xr:uid="{7DF67D48-D63D-43C5-9073-DA098A501C27}">
       <formula1>"TEST,QA,DEV,PROD"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2774,7 +2929,7 @@
   <dimension ref="A1:BQ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3105,98 +3260,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
1021 US - updated
1021 US - updated
</commit_message>
<xml_diff>
--- a/PSPSProject/testData/testData.xlsx
+++ b/PSPSProject/testData/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9276799-5832-4CB9-B791-0417AB13650E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CBC66D-CCA4-471C-9D57-6E3D3EDFD227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>Execute</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>Device Cache Logic</t>
+  </si>
+  <si>
+    <t>test_data_create_circuit_info_file.py</t>
+  </si>
+  <si>
+    <t>Circuit Info File Generation Logic</t>
+  </si>
+  <si>
+    <t>timeplace</t>
+  </si>
+  <si>
+    <t>2020-11-07-V-01</t>
   </si>
 </sst>
 </file>
@@ -740,7 +752,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1836,41 +1932,41 @@
   </sheetPr>
   <dimension ref="A1:GU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.109375" style="39" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.109375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="38" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.44140625" style="37" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="37" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="37" customWidth="1"/>
-    <col min="11" max="11" width="23.109375" style="37" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="37" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="37" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.140625" style="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.140625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="35" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" style="37" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="38" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" style="37" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="37" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="37" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="37" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="37" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="37" customWidth="1"/>
     <col min="14" max="14" width="21" style="34" customWidth="1"/>
-    <col min="15" max="92" width="9.109375" style="34"/>
-    <col min="93" max="147" width="9.109375" style="35"/>
-    <col min="148" max="148" width="9.109375" style="35" collapsed="1"/>
-    <col min="149" max="186" width="9.109375" style="35"/>
-    <col min="187" max="187" width="9.109375" style="35" collapsed="1"/>
-    <col min="188" max="191" width="9.109375" style="35"/>
-    <col min="192" max="192" width="9.109375" style="35" collapsed="1"/>
-    <col min="193" max="194" width="9.109375" style="35"/>
-    <col min="195" max="195" width="9.109375" style="35" collapsed="1"/>
-    <col min="196" max="203" width="9.109375" style="35"/>
-    <col min="204" max="16384" width="9.109375" style="35" collapsed="1"/>
+    <col min="15" max="92" width="9.140625" style="34"/>
+    <col min="93" max="147" width="9.140625" style="35"/>
+    <col min="148" max="148" width="9.140625" style="35" collapsed="1"/>
+    <col min="149" max="186" width="9.140625" style="35"/>
+    <col min="187" max="187" width="9.140625" style="35" collapsed="1"/>
+    <col min="188" max="191" width="9.140625" style="35"/>
+    <col min="192" max="192" width="9.140625" style="35" collapsed="1"/>
+    <col min="193" max="194" width="9.140625" style="35"/>
+    <col min="195" max="195" width="9.140625" style="35" collapsed="1"/>
+    <col min="196" max="203" width="9.140625" style="35"/>
+    <col min="204" max="16384" width="9.140625" style="35" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:92" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1968,7 +2064,7 @@
       <c r="CM1" s="2"/>
       <c r="CN1" s="2"/>
     </row>
-    <row r="2" spans="1:92" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:92" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -2062,7 +2158,7 @@
       <c r="CM2" s="2"/>
       <c r="CN2" s="2"/>
     </row>
-    <row r="3" spans="1:92" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:92" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -2109,7 +2205,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:92" s="34" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:92" s="34" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -2174,7 +2270,7 @@
       <c r="AP4" s="33"/>
       <c r="AQ4" s="33"/>
     </row>
-    <row r="5" spans="1:92" s="34" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:92" s="34" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -2241,7 +2337,7 @@
       <c r="AP5" s="33"/>
       <c r="AQ5" s="33"/>
     </row>
-    <row r="6" spans="1:92" s="34" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:92" s="34" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
@@ -2306,7 +2402,7 @@
       <c r="AP6" s="33"/>
       <c r="AQ6" s="33"/>
     </row>
-    <row r="7" spans="1:92" s="34" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:92" s="34" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
@@ -2369,7 +2465,7 @@
       <c r="AP7" s="33"/>
       <c r="AQ7" s="33"/>
     </row>
-    <row r="8" spans="1:92" s="2" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:92" s="2" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>7</v>
       </c>
@@ -2389,130 +2485,130 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="71" priority="381" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="382" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="381" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="382" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="69" priority="379" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="380" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="379" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="380" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="67" priority="377" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="377" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="378" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="65" priority="375" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="376" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="375" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="376" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="63" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="59" priority="19" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="57" priority="17" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="55" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="16" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="53" priority="13" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2542,36 +2638,37 @@
   </sheetPr>
   <dimension ref="A1:GV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.109375" style="39" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.109375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="39" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.140625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="35" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" style="37" customWidth="1"/>
     <col min="6" max="6" width="12" style="38" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="86" width="9.109375" style="34"/>
-    <col min="87" max="141" width="9.109375" style="35"/>
-    <col min="142" max="142" width="9.109375" style="35" collapsed="1"/>
-    <col min="143" max="180" width="9.109375" style="35"/>
-    <col min="181" max="181" width="9.109375" style="35" collapsed="1"/>
-    <col min="182" max="185" width="9.109375" style="35"/>
-    <col min="186" max="186" width="9.109375" style="35" collapsed="1"/>
-    <col min="187" max="188" width="9.109375" style="35"/>
-    <col min="189" max="189" width="9.109375" style="35" collapsed="1"/>
-    <col min="190" max="197" width="9.109375" style="35"/>
-    <col min="198" max="198" width="9.109375" style="35" collapsed="1"/>
-    <col min="199" max="204" width="9.109375" style="35"/>
-    <col min="205" max="16384" width="9.109375" style="35" collapsed="1"/>
+    <col min="7" max="7" width="26.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="86" width="9.140625" style="34"/>
+    <col min="87" max="141" width="9.140625" style="35"/>
+    <col min="142" max="142" width="9.140625" style="35" collapsed="1"/>
+    <col min="143" max="180" width="9.140625" style="35"/>
+    <col min="181" max="181" width="9.140625" style="35" collapsed="1"/>
+    <col min="182" max="185" width="9.140625" style="35"/>
+    <col min="186" max="186" width="9.140625" style="35" collapsed="1"/>
+    <col min="187" max="188" width="9.140625" style="35"/>
+    <col min="189" max="189" width="9.140625" style="35" collapsed="1"/>
+    <col min="190" max="197" width="9.140625" style="35"/>
+    <col min="198" max="198" width="9.140625" style="35" collapsed="1"/>
+    <col min="199" max="204" width="9.140625" style="35"/>
+    <col min="205" max="16384" width="9.140625" style="35" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2584,8 +2681,9 @@
       <c r="F1" s="50"/>
       <c r="G1" s="51"/>
       <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
     </row>
-    <row r="2" spans="1:8" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
@@ -2594,8 +2692,9 @@
       <c r="F2" s="54"/>
       <c r="G2" s="27"/>
       <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
     </row>
-    <row r="3" spans="1:8" s="34" customFormat="1" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" s="34" customFormat="1" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -2620,8 +2719,11 @@
       <c r="H3" s="21" t="s">
         <v>9</v>
       </c>
+      <c r="I3" s="21" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -2644,8 +2746,9 @@
         <v>45</v>
       </c>
       <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
     </row>
-    <row r="5" spans="1:8" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -2668,25 +2771,81 @@
         <v>45</v>
       </c>
       <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="24"/>
       <c r="G7" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="37" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="20" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2694,7 +2853,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2702,7 +2861,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2710,7 +2869,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5">
     <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2718,7 +2877,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A6">
     <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2726,7 +2885,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A6">
     <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2734,7 +2893,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A6">
     <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2742,7 +2901,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A6">
     <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2751,16 +2910,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A5" xr:uid="{97BE53CD-10F5-4B65-A481-D9129253028C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6" xr:uid="{97BE53CD-10F5-4B65-A481-D9129253028C}">
       <formula1>"Y,N,End"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CCDA7A78-A04D-4402-B991-2E5BCAB586CA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F6" xr:uid="{CCDA7A78-A04D-4402-B991-2E5BCAB586CA}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D5" xr:uid="{26455790-AA52-4327-A83D-3E6CDDE2F64E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D6" xr:uid="{26455790-AA52-4327-A83D-3E6CDDE2F64E}">
       <formula1>"Chrome-Default,Chrome-Headless,Chrome-MAC-Default,Chrome-MAC-Headless"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E5" xr:uid="{7DF67D48-D63D-43C5-9073-DA098A501C27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E6" xr:uid="{7DF67D48-D63D-43C5-9073-DA098A501C27}">
       <formula1>"TEST,QA,DEV,PROD"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2777,23 +2936,23 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="44"/>
-    <col min="2" max="2" width="35.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="44" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="44"/>
-    <col min="6" max="6" width="8.5546875" style="44" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" style="44" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="44"/>
+    <col min="2" max="2" width="35.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="44" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="44"/>
+    <col min="6" max="6" width="8.5703125" style="44" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="44" customWidth="1"/>
     <col min="11" max="11" width="10" style="44" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="44"/>
+    <col min="12" max="16384" width="8.85546875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="35" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:69" s="35" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2868,7 +3027,7 @@
       <c r="BP1" s="34"/>
       <c r="BQ1" s="34"/>
     </row>
-    <row r="2" spans="1:69" s="35" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:69" s="35" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
@@ -2939,7 +3098,7 @@
       <c r="BP2" s="34"/>
       <c r="BQ2" s="34"/>
     </row>
-    <row r="3" spans="1:69" s="34" customFormat="1" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:69" s="34" customFormat="1" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -2974,7 +3133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:69" s="34" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" s="34" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -3026,7 +3185,7 @@
       <c r="AG4" s="33"/>
       <c r="AH4" s="33"/>
     </row>
-    <row r="5" spans="1:69" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:69" s="34" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -3078,7 +3237,7 @@
       <c r="AG5" s="33"/>
       <c r="AH5" s="33"/>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
@@ -3227,20 +3386,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -3321,7 +3480,7 @@
       <c r="BV1" s="2"/>
       <c r="BW1" s="2"/>
     </row>
-    <row r="2" spans="1:75" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -3398,7 +3557,7 @@
       <c r="BV2" s="2"/>
       <c r="BW2" s="2"/>
     </row>
-    <row r="3" spans="1:75" s="2" customFormat="1" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" s="2" customFormat="1" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -3436,7 +3595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:75" s="2" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:75" s="2" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>7</v>
       </c>
@@ -3454,23 +3613,23 @@
       <c r="M4" s="47"/>
       <c r="N4" s="47"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K6" s="44"/>
       <c r="L6" s="44"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K7" s="44"/>
       <c r="L7" s="44"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K8" s="44"/>
       <c r="L8" s="44"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K9" s="44"/>
       <c r="L9" s="44"/>
     </row>

</xml_diff>

<commit_message>
Updated isolation zone script
</commit_message>
<xml_diff>
--- a/PSPSProject/testData/testData.xlsx
+++ b/PSPSProject/testData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B5450B-0D12-48BD-A6C3-F05C0C2EB4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849B225E-64C0-4299-A3C9-60897194C9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
   <si>
     <t>Execute</t>
   </si>
@@ -253,9 +253,6 @@
   </si>
   <si>
     <t>2020-14-10-TP-01</t>
-  </si>
-  <si>
-    <t>Auto_TP_20210202_104759</t>
   </si>
   <si>
     <t>245Cir_Polygon</t>
@@ -2810,7 +2807,7 @@
   <dimension ref="A1:GV23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2920,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
@@ -2946,12 +2943,12 @@
         <v>1</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:86" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
@@ -2974,12 +2971,12 @@
         <v>1</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="46"/>
       <c r="J6" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:86" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
@@ -3002,7 +2999,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="46"/>
       <c r="I7" s="46" t="s">
@@ -3032,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="46" t="s">
@@ -3064,7 +3061,7 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" s="33" t="s">
         <v>72</v>
@@ -3075,10 +3072,10 @@
       <c r="E12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J12" s="33" t="s">
         <v>73</v>
@@ -3090,10 +3087,10 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="33" t="s">
         <v>77</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:86" x14ac:dyDescent="0.3">
@@ -3102,7 +3099,7 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>70</v>
@@ -3114,10 +3111,10 @@
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:86" x14ac:dyDescent="0.3">
@@ -3126,10 +3123,10 @@
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="33" t="s">
         <v>82</v>
-      </c>
-      <c r="J16" s="33" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
@@ -3139,10 +3136,10 @@
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
@@ -3155,7 +3152,7 @@
         <v>62</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update for dev env
</commit_message>
<xml_diff>
--- a/PSPSProject/testData/testData.xlsx
+++ b/PSPSProject/testData/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849B225E-64C0-4299-A3C9-60897194C9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE45169-6919-46FC-B236-8152BE6614C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>Execute</t>
   </si>
@@ -213,9 +213,6 @@
     <t>test_data_defaultdevicecheck.py</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>defaultcircuits_output.csv</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
     <t>2020-14-10-TP-01</t>
   </si>
   <si>
+    <t>Auto_TP_20210202_104759</t>
+  </si>
+  <si>
     <t>245Cir_Polygon</t>
   </si>
   <si>
@@ -294,17 +294,35 @@
     <t>Auto_TP_20210202_141853</t>
   </si>
   <si>
-    <t>2020-11-04-TP-01</t>
-  </si>
-  <si>
-    <t>18MAYTP1_Polygon_auto</t>
+    <t>2021-09-08-TP-01</t>
+  </si>
+  <si>
+    <t>0224_Normalcircuit_SmokeTest</t>
+  </si>
+  <si>
+    <t>tst-123</t>
+  </si>
+  <si>
+    <t>test_psps_ui_create_event.py</t>
+  </si>
+  <si>
+    <t>Time places,Stage,Status,Tied to event,Created by,Last modified,External name</t>
+  </si>
+  <si>
+    <t>Create event</t>
+  </si>
+  <si>
+    <t>Event validate circuit file</t>
+  </si>
+  <si>
+    <t>test_psps_ui_eventmanagement_circuit_validation.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +439,20 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -667,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -831,12 +863,183 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="104">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2098,43 +2301,43 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:GU8"/>
+  <dimension ref="A1:GU10"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="36" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.109375" style="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.109375" style="34" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="34" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="37" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.44140625" style="36" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="36" customWidth="1"/>
-    <col min="11" max="11" width="23.109375" style="36" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="36" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="36" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.140625" style="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.140625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="34" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" style="36" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="37" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" style="36" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="36" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="36" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="36" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="36" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="36" customWidth="1"/>
     <col min="14" max="14" width="21" style="33" customWidth="1"/>
-    <col min="15" max="92" width="9.109375" style="33"/>
-    <col min="93" max="147" width="9.109375" style="34"/>
-    <col min="148" max="148" width="9.109375" style="34" collapsed="1"/>
-    <col min="149" max="186" width="9.109375" style="34"/>
-    <col min="187" max="187" width="9.109375" style="34" collapsed="1"/>
-    <col min="188" max="191" width="9.109375" style="34"/>
-    <col min="192" max="192" width="9.109375" style="34" collapsed="1"/>
-    <col min="193" max="194" width="9.109375" style="34"/>
-    <col min="195" max="195" width="9.109375" style="34" collapsed="1"/>
-    <col min="196" max="203" width="9.109375" style="34"/>
-    <col min="204" max="16384" width="9.109375" style="34" collapsed="1"/>
+    <col min="15" max="92" width="9.140625" style="33"/>
+    <col min="93" max="147" width="9.140625" style="34"/>
+    <col min="148" max="148" width="9.140625" style="34" collapsed="1"/>
+    <col min="149" max="186" width="9.140625" style="34"/>
+    <col min="187" max="187" width="9.140625" style="34" collapsed="1"/>
+    <col min="188" max="191" width="9.140625" style="34"/>
+    <col min="192" max="192" width="9.140625" style="34" collapsed="1"/>
+    <col min="193" max="194" width="9.140625" style="34"/>
+    <col min="195" max="195" width="9.140625" style="34" collapsed="1"/>
+    <col min="196" max="203" width="9.140625" style="34"/>
+    <col min="204" max="16384" width="9.140625" style="34" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:92" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2232,7 +2435,7 @@
       <c r="CM1" s="2"/>
       <c r="CN1" s="2"/>
     </row>
-    <row r="2" spans="1:92" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:92" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -2326,7 +2529,7 @@
       <c r="CM2" s="2"/>
       <c r="CN2" s="2"/>
     </row>
-    <row r="3" spans="1:92" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:92" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -2373,7 +2576,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:92" s="33" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:92" s="33" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -2387,14 +2590,14 @@
         <v>17</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F4" s="42">
         <v>1</v>
       </c>
       <c r="G4" s="46"/>
       <c r="H4" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" s="47"/>
       <c r="J4" s="47" t="s">
@@ -2438,7 +2641,7 @@
       <c r="AP4" s="32"/>
       <c r="AQ4" s="32"/>
     </row>
-    <row r="5" spans="1:92" s="33" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:92" s="33" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -2452,14 +2655,14 @@
         <v>17</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F5" s="42">
         <v>1</v>
       </c>
       <c r="G5" s="46"/>
       <c r="H5" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" s="47" t="s">
         <v>36</v>
@@ -2505,7 +2708,7 @@
       <c r="AP5" s="32"/>
       <c r="AQ5" s="32"/>
     </row>
-    <row r="6" spans="1:92" s="33" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:92" s="33" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
@@ -2519,14 +2722,14 @@
         <v>17</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F6" s="42">
         <v>1</v>
       </c>
       <c r="G6" s="46"/>
       <c r="H6" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" s="47"/>
       <c r="J6" s="47" t="s">
@@ -2570,7 +2773,7 @@
       <c r="AP6" s="32"/>
       <c r="AQ6" s="32"/>
     </row>
-    <row r="7" spans="1:92" s="33" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:92" s="33" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
@@ -2584,7 +2787,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F7" s="42">
         <v>1</v>
@@ -2633,90 +2836,284 @@
       <c r="AP7" s="32"/>
       <c r="AQ7" s="32"/>
     </row>
-    <row r="8" spans="1:92" s="2" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="42"/>
+    <row r="8" spans="1:92" s="33" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="42">
+        <v>1</v>
+      </c>
       <c r="G8" s="46"/>
       <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="47" t="s">
+        <v>91</v>
+      </c>
       <c r="L8" s="46"/>
       <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
+      <c r="N8" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="47"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="32"/>
+      <c r="AJ8" s="32"/>
+      <c r="AK8" s="32"/>
+      <c r="AL8" s="32"/>
+      <c r="AM8" s="32"/>
+      <c r="AN8" s="32"/>
+      <c r="AO8" s="32"/>
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="32"/>
+    </row>
+    <row r="9" spans="1:92" s="33" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="42">
+        <v>1</v>
+      </c>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="47"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
+      <c r="AA9" s="32"/>
+      <c r="AB9" s="32"/>
+      <c r="AC9" s="32"/>
+      <c r="AD9" s="32"/>
+      <c r="AE9" s="32"/>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="32"/>
+      <c r="AH9" s="32"/>
+      <c r="AI9" s="32"/>
+      <c r="AJ9" s="32"/>
+      <c r="AK9" s="32"/>
+      <c r="AL9" s="32"/>
+      <c r="AM9" s="32"/>
+      <c r="AN9" s="32"/>
+      <c r="AO9" s="32"/>
+      <c r="AP9" s="32"/>
+      <c r="AQ9" s="32"/>
+    </row>
+    <row r="10" spans="1:92" s="2" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="87" priority="381" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="382" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="405" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="406" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="85" priority="379" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="380" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="403" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="404" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="83" priority="377" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="401" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="402" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="81" priority="375" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="376" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="399" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="400" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="79" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="47" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="48" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="45" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="46" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="75" priority="19" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="43" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="44" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="73" priority="17" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="41" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="87" priority="39" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="40" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="85" priority="37" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="38" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="83" priority="35" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="36" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="81" priority="33" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="34" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="79" priority="31" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="32" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="77" priority="29" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="30" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="75" priority="27" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="73" priority="25" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="26" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
     <cfRule type="cellIs" dxfId="71" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2724,7 +3121,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
+  <conditionalFormatting sqref="A8">
     <cfRule type="cellIs" dxfId="69" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2732,7 +3129,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
+  <conditionalFormatting sqref="A8">
     <cfRule type="cellIs" dxfId="67" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2740,7 +3137,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
+  <conditionalFormatting sqref="A8">
     <cfRule type="cellIs" dxfId="65" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2748,7 +3145,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="63" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2756,7 +3153,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="61" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2764,7 +3161,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="59" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2772,7 +3169,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2781,16 +3178,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7" xr:uid="{3B1CCEEA-3289-44C8-9D1D-04599A1B1D40}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E9" xr:uid="{3B1CCEEA-3289-44C8-9D1D-04599A1B1D40}">
       <formula1>"TEST,QA,DEV,PROD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D7" xr:uid="{2C0620C3-AC94-442D-A0A9-232665619B8E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D9" xr:uid="{2C0620C3-AC94-442D-A0A9-232665619B8E}">
       <formula1>"Chrome-Default,Chrome-Headless,Chrome-MAC-Default,Chrome-MAC-Headless"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7" xr:uid="{5B503B92-99F5-49E9-AAB9-A55EE2349403}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F9" xr:uid="{5B503B92-99F5-49E9-AAB9-A55EE2349403}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A7" xr:uid="{6EA13E7D-46C4-4E6E-8A6E-850237CC6134}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A9" xr:uid="{6EA13E7D-46C4-4E6E-8A6E-850237CC6134}">
       <formula1>"Y,N,End"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2806,38 +3203,38 @@
   </sheetPr>
   <dimension ref="A1:GV23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="36" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.109375" style="38" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.109375" style="34" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="34" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="38" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.140625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="34" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" style="36" customWidth="1"/>
     <col min="6" max="6" width="12" style="37" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.77734375" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" style="33" customWidth="1"/>
-    <col min="11" max="85" width="9.109375" style="33"/>
-    <col min="86" max="140" width="9.109375" style="34"/>
-    <col min="141" max="141" width="9.109375" style="34" collapsed="1"/>
-    <col min="142" max="179" width="9.109375" style="34"/>
-    <col min="180" max="180" width="9.109375" style="34" collapsed="1"/>
-    <col min="181" max="184" width="9.109375" style="34"/>
-    <col min="185" max="185" width="9.109375" style="34" collapsed="1"/>
-    <col min="186" max="187" width="9.109375" style="34"/>
-    <col min="188" max="188" width="9.109375" style="34" collapsed="1"/>
-    <col min="189" max="196" width="9.109375" style="34"/>
-    <col min="197" max="197" width="9.109375" style="34" collapsed="1"/>
-    <col min="198" max="204" width="9.109375" style="34"/>
-    <col min="205" max="16384" width="9.109375" style="34" collapsed="1"/>
+    <col min="7" max="7" width="33.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="33" customWidth="1"/>
+    <col min="11" max="85" width="9.140625" style="33"/>
+    <col min="86" max="140" width="9.140625" style="34"/>
+    <col min="141" max="141" width="9.140625" style="34" collapsed="1"/>
+    <col min="142" max="179" width="9.140625" style="34"/>
+    <col min="180" max="180" width="9.140625" style="34" collapsed="1"/>
+    <col min="181" max="184" width="9.140625" style="34"/>
+    <col min="185" max="185" width="9.140625" style="34" collapsed="1"/>
+    <col min="186" max="187" width="9.140625" style="34"/>
+    <col min="188" max="188" width="9.140625" style="34" collapsed="1"/>
+    <col min="189" max="196" width="9.140625" style="34"/>
+    <col min="197" max="197" width="9.140625" style="34" collapsed="1"/>
+    <col min="198" max="204" width="9.140625" style="34"/>
+    <col min="205" max="16384" width="9.140625" style="34" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:86" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2853,7 +3250,7 @@
       <c r="I1" s="50"/>
       <c r="J1" s="50"/>
     </row>
-    <row r="2" spans="1:86" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:86" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -2865,7 +3262,7 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="1:86" s="33" customFormat="1" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:86" s="33" customFormat="1" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -2882,7 +3279,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" s="44" t="s">
         <v>57</v>
@@ -2891,13 +3288,13 @@
         <v>9</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:86" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:86" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -2911,7 +3308,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F4" s="42">
         <v>1</v>
@@ -2923,7 +3320,7 @@
       <c r="I4" s="46"/>
       <c r="J4" s="46"/>
     </row>
-    <row r="5" spans="1:86" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:86" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -2937,35 +3334,33 @@
         <v>17</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F5" s="42">
         <v>1</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="46"/>
-      <c r="J5" s="46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:86" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="56"/>
+    </row>
+    <row r="6" spans="1:86" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F6" s="42">
         <v>1</v>
@@ -2975,11 +3370,9 @@
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="46"/>
-      <c r="J6" s="46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:86" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="46"/>
+    </row>
+    <row r="7" spans="1:86" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
@@ -2993,7 +3386,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F7" s="42">
         <v>1</v>
@@ -3003,27 +3396,25 @@
       </c>
       <c r="H7" s="46"/>
       <c r="I7" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="J7" s="46"/>
+    </row>
+    <row r="8" spans="1:86" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F8" s="42">
         <v>1</v>
@@ -3033,28 +3424,26 @@
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="46" t="s">
-        <v>73</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="J8" s="46"/>
       <c r="CH8" s="33"/>
     </row>
-    <row r="9" spans="1:86" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:86" x14ac:dyDescent="0.25">
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:86" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:86" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -3064,10 +3453,10 @@
         <v>74</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:86" ht="27.6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:86" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
       <c r="G12" s="37"/>
@@ -3078,10 +3467,10 @@
         <v>75</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:86" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:86" x14ac:dyDescent="0.25">
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
       <c r="G13" s="37"/>
@@ -3093,7 +3482,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:86" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
       <c r="G14" s="37"/>
@@ -3102,10 +3491,10 @@
         <v>78</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:86" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
       <c r="D15" s="37"/>
       <c r="E15" s="37"/>
       <c r="G15" s="37"/>
@@ -3117,7 +3506,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:86" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
       <c r="G16" s="37"/>
@@ -3129,7 +3518,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C17" s="54"/>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
@@ -3142,54 +3531,61 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C18" s="55"/>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C19" s="55"/>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C20" s="55"/>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
-    </row>
-    <row r="21" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="J20" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C21" s="55"/>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="3:10" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C22" s="55"/>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="J22" s="46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="A4">
     <cfRule type="cellIs" dxfId="55" priority="31" operator="equal">
       <formula>"Y"</formula>
@@ -3345,23 +3741,23 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="43"/>
-    <col min="2" max="2" width="35.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="43" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="43"/>
-    <col min="6" max="6" width="8.5546875" style="43" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" style="43" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="43"/>
+    <col min="2" max="2" width="35.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="43"/>
+    <col min="6" max="6" width="8.5703125" style="43" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="43" customWidth="1"/>
     <col min="11" max="11" width="10" style="43" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="43"/>
+    <col min="12" max="16384" width="8.85546875" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="34" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:69" s="34" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -3436,7 +3832,7 @@
       <c r="BP1" s="33"/>
       <c r="BQ1" s="33"/>
     </row>
-    <row r="2" spans="1:69" s="34" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:69" s="34" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -3507,7 +3903,7 @@
       <c r="BP2" s="33"/>
       <c r="BQ2" s="33"/>
     </row>
-    <row r="3" spans="1:69" s="33" customFormat="1" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:69" s="33" customFormat="1" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -3542,7 +3938,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:69" s="33" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" s="33" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -3594,7 +3990,7 @@
       <c r="AG4" s="32"/>
       <c r="AH4" s="32"/>
     </row>
-    <row r="5" spans="1:69" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:69" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -3646,7 +4042,7 @@
       <c r="AG5" s="32"/>
       <c r="AH5" s="32"/>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
@@ -3795,20 +4191,20 @@
       <selection activeCell="C16" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -3889,7 +4285,7 @@
       <c r="BV1" s="2"/>
       <c r="BW1" s="2"/>
     </row>
-    <row r="2" spans="1:75" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -3966,7 +4362,7 @@
       <c r="BV2" s="2"/>
       <c r="BW2" s="2"/>
     </row>
-    <row r="3" spans="1:75" s="2" customFormat="1" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" s="2" customFormat="1" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -4004,7 +4400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:75" s="2" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:75" s="2" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>7</v>
       </c>
@@ -4022,23 +4418,23 @@
       <c r="M4" s="46"/>
       <c r="N4" s="46"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K5" s="43"/>
       <c r="L5" s="43"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K6" s="43"/>
       <c r="L6" s="43"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K8" s="43"/>
       <c r="L8" s="43"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
     </row>

</xml_diff>